<commit_message>
Updated Aerosol for MIROC6, citation and parties.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_miroc_citations.xlsx
+++ b/cmip6/citations/cmip6_miroc_citations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipsl/Engineering/esdoc/bash/cmip6/citations/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Documents/work/project/CMIP6/ES-DOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3B9249-E2A6-2448-9F22-74A155B1A05C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCF2095-8027-7240-A386-EE25EBF2ECB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -62,31 +62,116 @@
     <t>10.1002/2013JD020445</t>
   </si>
   <si>
+    <t>BibTex</t>
+  </si>
+  <si>
+    <t>http://journal.com/873487234</t>
+  </si>
+  <si>
+    <t>Nativi_2008</t>
+  </si>
+  <si>
+    <t>Long name for internal use (unarchived)</t>
+  </si>
+  <si>
+    <t>SPRINTARS_T</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>10.1029/2000JD900265</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/abs/10.1029/2000JD900265</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
     <t>"@article{
   title = {Unidata's Common Data Model Mapping to the ISO 19123 Data Model},
   journal = {Earth Science Informatics},
   author = {Nativi, Stefano and Caron, John and Domenico, Ben and Bigagli, Lorenzo},
   year = {2008},
 }"</t>
-  </si>
-  <si>
-    <t>BibTex</t>
-  </si>
-  <si>
-    <t>http://journal.com/873487234</t>
-  </si>
-  <si>
-    <t>Nativi_2008</t>
-  </si>
-  <si>
-    <t>Long name for internal use (unarchived)</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {Global three-dimensional simulation of aerosol optical thickness distribution of various origins},
+  journal = {Journal of Geophysical Research},
+  author = {Takemura, Toshihiko and Okamoto, Hajime and Maruyama, Yoshihiro and Numaguti, Atusi and Higurashi, Akiko and Nakajima, Teruyuki},
+  year = {2000},
+}"</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>10.1175/1520-0442(2002)015&lt;0333:SSAARF&gt;2.0.CO;2</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/abs/10.1175/1520-0442(2002)015%3C0333%3ASSAARF%3E2.0.CO;2</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {Single-scattering albedo and radiative forcing of various aerosol species with a global three-dimensional model},
+  journal = {Journal of Climate},
+  author = {Takemura, Toshihiko and Nakajima, Teruyuki and Dubovik, Oleg and Holben, Brent N. and Kinne, Stefan},
+  year = {2002},
+}"</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>SPRINTARS_R</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>SPRINTARS_C</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>10.1029/2004JD005029</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {Simulation of climate response to aerosol direct and indirect effects with aerosol transport-radiation model},
+  journal = {Journal of Geophysical Research},
+  author = {Takemura, Toshihiko and Nozawa, Toru and Emori, Seita and Nakajima, Takashi Y. and Nakajima, Teruyuki},
+  year = {2005},
+}"</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2004JD005029</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>SPRINTARS_M</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>https://www.atmos-chem-phys.net/9/3061/2009/acp-9-3061-2009.html</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>10.5194/acp-9-3061-2009</t>
+    <phoneticPr fontId="11"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {A simulation of the global distribution and radiative forcing of soil dust aerosols at the Last Glacial Maximum},
+  journal = {Atmospheric Chemistry and Physics},
+  author = {Takemura, Toshihiko and Egashira, Mio and Matsuzawa, Kanako and Ichijo, Hironori and O'ishi, Ryota and Abe-Ouchi, Ayako},
+  year = {2009},
+}"</t>
+    <phoneticPr fontId="11"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -153,6 +238,18 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="A-OTF Futo Go B101 Pr6N Bold"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="4">
@@ -293,7 +390,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -376,9 +473,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1535,9 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
@@ -1545,7 +1648,7 @@
     <col min="6" max="256" width="8.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="34.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1554,14 +1657,14 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="25.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1572,14 +1675,14 @@
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="25.5" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1590,14 +1693,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="409" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="409" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1605,6 +1708,7 @@
       <c r="E7" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -1623,9 +1727,11 @@
   </sheetPr>
   <dimension ref="A1:IP56"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26.83203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" style="10" customWidth="1"/>
@@ -1635,7 +1741,7 @@
     <col min="6" max="250" width="16.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:250" ht="31" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1750,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="20.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -1652,27 +1758,27 @@
         <v>8</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:250" s="27" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:250" s="27" customFormat="1" ht="129" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="25"/>
       <c r="F3" s="26"/>
@@ -1921,371 +2027,371 @@
       <c r="IO3" s="26"/>
       <c r="IP3" s="26"/>
     </row>
-    <row r="4" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:250" ht="20" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:250" ht="20" customHeight="1">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:250" ht="20" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:250" ht="20" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:250" ht="20" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:250" ht="20" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:250" ht="20" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:250" ht="20" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:250" ht="20" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:250" ht="20" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:250" ht="20" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:250" ht="20" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:250" ht="20" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
     </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="20" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="20" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="20" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="20" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="20" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="20" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="20" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="20" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="20" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="20" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="20" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="20" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="20" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="20" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="20" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="20" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="20" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="20" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="20" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="20" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="20" customHeight="1">
       <c r="A53" s="17"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="20" customHeight="1">
       <c r="A54" s="17"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="20" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="20" customHeight="1">
       <c r="A56" s="17"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -2293,6 +2399,7 @@
       <c r="E56" s="22"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -2308,9 +2415,11 @@
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26.83203125" style="18" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" style="18" customWidth="1"/>
@@ -2320,7 +2429,7 @@
     <col min="6" max="250" width="16.33203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:250" ht="31" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2329,7 +2438,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="20.75" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
@@ -2337,13 +2446,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="IK2"/>
       <c r="IL2"/>
@@ -2352,350 +2461,382 @@
       <c r="IO2"/>
       <c r="IP2"/>
     </row>
-    <row r="3" spans="1:250" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+    <row r="3" spans="1:250" ht="136">
+      <c r="A3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+    <row r="4" spans="1:250" ht="136">
+      <c r="A4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+    <row r="5" spans="1:250" ht="136">
+      <c r="A5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+    <row r="6" spans="1:250" ht="136">
+      <c r="A6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:250" ht="20" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:250" ht="20" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:250" ht="20" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:250" ht="20" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:250" ht="20" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:250" ht="20" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:250" ht="20" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:250" ht="20" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:250" ht="20" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:250" ht="20" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="20" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="20" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="20" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="20" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="20" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="20" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="20" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="20" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="20" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="20" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="20" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="20" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="20" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="20" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="20" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="20" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="20" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="20" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="20" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="20" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="20" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="20" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="20" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="20" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="20" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="20" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="20" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="20" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="20" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="20" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
@@ -2703,6 +2844,7 @@
       <c r="E52" s="22"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Upload Atmoschem for MIROC-ES2H, citation and parties, turn "on" to publish.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_miroc_citations.xlsx
+++ b/cmip6/citations/cmip6_miroc_citations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toshi/Documents/work/project/CMIP6/ES-DOC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Takahiro\Google ドライブ\ES-DOC\collected\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCF2095-8027-7240-A386-EE25EBF2ECB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21705" windowHeight="12975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -166,12 +165,101 @@
 }"</t>
     <phoneticPr fontId="11"/>
   </si>
+  <si>
+    <t>Akiyoshi_2009</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>10.1029/2007JD009261</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {A  CCM  simulation  of  the  breakup of  the  Antarctic  polar  vortex  in  the  years  1980–2004  under  the  CCMVal  scenarios},
+  journal = {J. Geophys. Res.},
+  author = {Akiyoshi, H., Zhou, L. B., Yamashita, Y., Sakamoto, K., Yoshiki, M.,  Nagashima,  T.,  Takahashi,  M.,  Kurokawa,  J.,  Takigawa, M.,  and  Imamura,  T.},
+  year = {2009},
+}"</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2007JD009261</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Watanabe_2011</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>10.5194/gmd-4-845-2011</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {MIROC-ESM 2010: model description and basic results of CMIP5-20c3m experiments},
+  journal = {Geosci. Model Dev.},
+  author = {Watanabe, S., Hajima, T., Sudo,K., Nagashima, T., Takemura, T., Okajima, H., Nozawa, T., Kawase, H., Abe, M., Yokohata, T., Ise, T., Sato, H., Kato, E., Takata, K., Emori, S., and Kawamiya, M.},
+  year = {2011},
+}"</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>https://www.geosci-model-dev.net/4/845/2011/gmd-4-845-2011.html</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Morgenstern_2017</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>10.5194/gmd-4-845-2011</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>@Article{gmd-10-639-2017,
+AUTHOR = {Morgenstern, O. and Hegglin, M. I. and Rozanov, E. and O'Connor, F. M. and Abraham, N. L. and Akiyoshi, H. and Archibald, A. T. and Bekki, S. and Butchart, N. and Chipperfield, M. P. and Deushi, M. and Dhomse, S. S. and Garcia, R. R. and Hardiman, S. C. and Horowitz, L. W. and J\"ockel, P. and Josse, B. and Kinnison, D. and Lin, M. and Mancini, E. and Manyin, M. E. and Marchand, M. and Mar\'ecal, V. and Michou, M. and Oman, L. D. and Pitari, G. and Plummer, D. A. and Revell, L. E. and Saint-Martin, D. and Schofield, R. and Stenke, A. and Stone, K. and Sudo, K. and Tanaka, T. Y. and Tilmes, S. and Yamashita, Y. and Yoshida, K. and Zeng, G.},
+TITLE = {Review of the global models used within {phase 1 of} the Chemistry--Climate Model Initiative (CCMI)},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {10},
+YEAR = {2017},
+NUMBER = {2},
+PAGES = {639--671},
+URL = {https://www.geosci-model-dev.net/10/639/2017/},
+DOI = {10.5194/gmd-10-639-2017}
+}</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>https://www.geosci-model-dev.net/10/639/2017/</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>Sudo_2002</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>10.1029/2001JD001113</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>"@article{
+  title = {CHASER: A global chemical model of the troposphere 1. Model description},
+  journal = {J. Geophys. Res.},
+  author = {Sudo, K., M. Takahashi, J. Kurokawa, and H. Akimoto},
+  year = {2002},
+}"</t>
+    <phoneticPr fontId="13"/>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2001JD001113</t>
+    <phoneticPr fontId="13"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -248,6 +336,20 @@
     <font>
       <sz val="6"/>
       <name val="A-OTF Futo Go B101 Pr6N Bold"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
@@ -385,12 +487,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -479,8 +584,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1635,20 +1744,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.1640625" style="1" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.25" customHeight="1">
+    <row r="1" spans="1:5" ht="34.35" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1693,14 +1802,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="409" customHeight="1">
+    <row r="6" spans="1:5" ht="408.95" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="409" customHeight="1">
+    <row r="7" spans="1:5" ht="408.95" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1710,7 +1819,7 @@
   </sheetData>
   <phoneticPr fontId="11"/>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1721,7 +1830,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1731,17 +1840,17 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="81.83203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="42.83203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="18" customWidth="1"/>
-    <col min="6" max="250" width="16.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="18" customWidth="1"/>
+    <col min="6" max="250" width="16.28515625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1">
+    <row r="1" spans="1:250" ht="30.95" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1859,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1">
+    <row r="2" spans="1:250" ht="20.85" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -2027,371 +2136,371 @@
       <c r="IO3" s="26"/>
       <c r="IP3" s="26"/>
     </row>
-    <row r="4" spans="1:250" ht="20" customHeight="1">
+    <row r="4" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:250" ht="20" customHeight="1">
+    <row r="5" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:250" ht="20" customHeight="1">
+    <row r="6" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1">
+    <row r="7" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1">
+    <row r="8" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1">
+    <row r="9" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1">
+    <row r="10" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1">
+    <row r="11" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1">
+    <row r="12" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1">
+    <row r="13" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1">
+    <row r="14" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1">
+    <row r="15" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1">
+    <row r="16" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
     </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1">
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1">
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1">
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1">
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1">
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1">
+    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1">
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1">
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1">
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1">
+    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1">
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1">
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1">
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1">
+    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1">
+    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1">
+    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1">
+    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1">
+    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1">
+    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:5" ht="20" customHeight="1">
+    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="17"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:5" ht="20" customHeight="1">
+    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="17"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5" ht="20" customHeight="1">
+    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="56" spans="1:5" ht="20" customHeight="1">
+    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="17"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -2409,27 +2518,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="81.83203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="42.83203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="18" customWidth="1"/>
-    <col min="6" max="250" width="16.33203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="18" customWidth="1"/>
+    <col min="6" max="250" width="16.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1">
+    <row r="1" spans="1:250" ht="30.95" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2438,7 +2547,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1">
+    <row r="2" spans="1:250" ht="20.85" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
@@ -2461,7 +2570,7 @@
       <c r="IO2"/>
       <c r="IP2"/>
     </row>
-    <row r="3" spans="1:250" ht="136">
+    <row r="3" spans="1:250" ht="128.25">
       <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
@@ -2476,7 +2585,7 @@
       </c>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:250" ht="136">
+    <row r="4" spans="1:250" ht="114">
       <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
@@ -2491,7 +2600,7 @@
       </c>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:250" ht="136">
+    <row r="5" spans="1:250" ht="114">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
@@ -2506,7 +2615,7 @@
       </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:250" ht="136">
+    <row r="6" spans="1:250" ht="114">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -2521,322 +2630,354 @@
       </c>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1">
+    <row r="7" spans="1:250" ht="139.5" customHeight="1">
+      <c r="A7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:250" ht="179.25" customHeight="1">
+      <c r="A8" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:250" ht="300" customHeight="1">
+      <c r="A9" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:250" ht="165" customHeight="1">
+      <c r="A10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1">
+    <row r="12" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1">
+    <row r="13" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1">
+    <row r="14" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1">
+    <row r="15" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1">
+    <row r="16" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1">
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1">
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1">
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1">
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1">
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1">
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1">
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1">
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1">
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1">
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1">
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1">
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1">
+    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1">
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1">
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1">
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1">
+    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1">
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1">
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1">
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1">
+    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1">
+    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1">
+    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1">
+    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1">
+    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1">
+    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
@@ -2845,6 +2986,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="11"/>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
Upload Land for MIROC6, citation and parties, turn "on" to publish.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_miroc_citations.xlsx
+++ b/cmip6/citations/cmip6_miroc_citations.xlsx
@@ -16,12 +16,15 @@
     <sheet name="Example" sheetId="2" r:id="rId2"/>
     <sheet name="Citations" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Citations!$A$1:$E$52</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -192,15 +195,6 @@
   </si>
   <si>
     <t>10.5194/gmd-4-845-2011</t>
-    <phoneticPr fontId="13"/>
-  </si>
-  <si>
-    <t>"@article{
-  title = {MIROC-ESM 2010: model description and basic results of CMIP5-20c3m experiments},
-  journal = {Geosci. Model Dev.},
-  author = {Watanabe, S., Hajima, T., Sudo,K., Nagashima, T., Takemura, T., Okajima, H., Nozawa, T., Kawase, H., Abe, M., Yokohata, T., Ise, T., Sato, H., Kato, E., Takata, K., Emori, S., and Kawamiya, M.},
-  year = {2011},
-}"</t>
     <phoneticPr fontId="13"/>
   </si>
   <si>
@@ -254,12 +248,210 @@
     <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1029/2001JD001113</t>
     <phoneticPr fontId="13"/>
   </si>
+  <si>
+    <t>Ngo_Duc_2007</t>
+  </si>
+  <si>
+    <t>10.5194/hessd-4-4389-2007</t>
+  </si>
+  <si>
+    <t>@Article{
+AUTHOR = {Ngo-Duc, T. and Oki, T. and Kanae, S.},
+TITLE = {A variable streamflow velocity method for global river routing model: model description and preliminary results},
+JOURNAL = {Hydrology and Earth System Sciences Discussions},
+VOLUME = {4},
+YEAR = {2007},
+PAGES = {4389--4414},
+}</t>
+  </si>
+  <si>
+    <t>https://www.hydrol-earth-syst-sci-discuss.net/hessd-2007-0182/</t>
+  </si>
+  <si>
+    <t>Nitta_2014</t>
+  </si>
+  <si>
+    <t>10.1175/JCLI-D-13-00310.1</t>
+  </si>
+  <si>
+    <t>@article{
+author = {Nitta, T. and Yoshimura, K. and Takata, K. and O’ishi, R. and Sueyoshi, T. and Kanae, S. and Oki, T. and Abe-Ouchi, A. and Liston, G. E.},
+title = {Representing Variability in Subgrid Snow Cover and Snow Depth in a Global Land Model: Offline Validation},
+journal = {Journal of Climate},
+volume = {27},
+number = {9},
+pages = {3318-3330},
+year = {2014},
+}</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/JCLI-D-13-00310.1</t>
+  </si>
+  <si>
+    <t>Nitta_2017</t>
+  </si>
+  <si>
+    <t>10.1175/JHM-D-16-0105.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@article{
+author = {Nitta, T. and Yoshimura, K. and Abe-Ouchi, A.},
+title = {Impact of Arctic Wetlands on the Climate System: Model Sensitivity Simulations with the MIROC5 AGCM and a Snow-Fed Wetland Scheme},
+journal = {Journal of Hydrometeorology},
+volume = {18},
+number = {11},
+pages = {2923-2936},
+year = {2017},
+}
+</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/JHM-D-16-0105.1</t>
+  </si>
+  <si>
+    <t>Oki_1998</t>
+  </si>
+  <si>
+    <t>10.1175/1087-3562(1998)002&lt;0001:DOTRIP&gt;2.3.CO;2</t>
+  </si>
+  <si>
+    <t>@article{
+author = {Oki, T. and Sud, Y. C.},
+title = {Design of Total Runoff Integrating Pathways (TRIP)—A Global River Channel Network},
+journal = {Earth Interactions},
+volume = {2},
+number = {1},
+pages = {1-37},
+year = {1998},
+}</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/1087-3562(1998)002&lt;0001:DOTRIP&gt;2.3.CO;2</t>
+  </si>
+  <si>
+    <t>Takata_2003</t>
+  </si>
+  <si>
+    <t>10.1016/S0921-8181(03)00030-4</t>
+  </si>
+  <si>
+    <t>@article{
+title = {Development of the minimal advanced treatments of surface interaction and runoff},
+journal = {Global and Planetary Change},
+volume = {38},
+number = {1},
+pages = {209 - 222},
+year = {2003},
+author = {Takata, K. and Emori, S. and Watanabe, T.},
+}</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0921818103000304</t>
+  </si>
+  <si>
+    <t>Watanabe_1994</t>
+  </si>
+  <si>
+    <t>10.1007/BF00712521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Article{
+author="Watanabe, T.",
+title="Bulk parameterization for a vegetated surface and its application to a simulation of nocturnal drainage flow",
+journal="Boundary-Layer Meteorology",
+year="1994",
+volume="70",
+number="1",
+pages="13--35",
+}
+</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF00712521</t>
+  </si>
+  <si>
+    <t>Watanabe_1995</t>
+  </si>
+  <si>
+    <t>10.2480/agrmet.51.57</t>
+  </si>
+  <si>
+    <t>@article{
+  title={A Simple Model of Shortwave-Radiation Transport within Canopy},
+  author={Watanabe, T. and Ohtani, Y.},
+  journal={Journal of Agricultural Meteorology},
+  volume={51},
+  number={1},
+  pages={57-60},
+  year={1995},
+}</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2480/agrmet.51.57</t>
+  </si>
+  <si>
+    <t>Yamazaki_2009</t>
+  </si>
+  <si>
+    <t>10.5194/hess-13-2241-2009</t>
+  </si>
+  <si>
+    <t>@Article{
+AUTHOR = {Yamazaki, D. and Oki, T. and Kanae, S.},
+TITLE = {Deriving a global river network map and its sub-grid topographic characteristics from a fine-resolution flow direction map},
+JOURNAL = {Hydrology and Earth System Sciences},
+VOLUME = {13},
+YEAR = {2009},
+NUMBER = {11},
+PAGES = {2241--2251},
+}</t>
+  </si>
+  <si>
+    <t>https://www.hydrol-earth-syst-sci.net/13/2241/2009/</t>
+  </si>
+  <si>
+    <t>Watanabe_2010</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>10.1175/2010JCLI3679.1</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t xml:space="preserve">@article{
+author = {Watanabe, Masahiro and Suzuki, Tatsuo and O’ishi, Ryouta and Komuro, Yoshiki and Watanabe, Shingo and Emori, Seita and Takemura, Toshihiko and Chikira, Minoru and Ogura, Tomoo and Sekiguchi, Miho and Takata, Kumiko and Yamazaki, Dai and Yokohata, Tokuta and Nozawa, Toru and Hasumi, Hiroyasu and Tatebe, Hiroaki and Kimoto, Masahide},
+title = {Improved Climate Simulation by MIROC5: Mean States, Variability, and Climate Sensitivity},
+journal = {Journal of Climate},
+year = {2010},
+volume = {23},
+number = {23},
+pages = {6312-6335},
+}
+</t>
+  </si>
+  <si>
+    <t>https://journals.ametsoc.org/doi/abs/10.1175/2010JCLI3679.1</t>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>@Article{
+AUTHOR = {Watanabe, S. and Hajima, T. and Sudo, K. and Nagashima, T. and Takemura, T. and Okajima, H. and Nozawa, T. and Kawase, H. and Abe, M. and Yokohata, T. and Ise, T. and Sato, H. and Kato, E. and Takata, K. and Emori, S. and Kawamiya, M.},
+TITLE = {MIROC-ESM 2010: model description and basic results of CMIP5-20c3m experiments},
+JOURNAL = {Geoscientific Model Development},
+VOLUME = {4},
+YEAR = {2011},
+NUMBER = {4},
+PAGES = {845--872},
+URL = {https://www.geosci-model-dev.net/4/845/2011/},
+DOI = {10.5194/gmd-4-845-2011}
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -350,6 +542,12 @@
     <font>
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="Akanesyotai-boku-"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
@@ -495,7 +693,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -585,6 +783,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2524,8 +2734,8 @@
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -2652,192 +2862,509 @@
       <c r="B8" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>38</v>
       </c>
       <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:250" ht="300" customHeight="1">
       <c r="A9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="C9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="D9" s="30" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>42</v>
       </c>
       <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:250" ht="165" customHeight="1">
       <c r="A10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="C10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="D10" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:250" ht="132" customHeight="1">
+      <c r="A11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="B11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:250" ht="161.1" customHeight="1">
+      <c r="A12" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:250" ht="141.94999999999999" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:250" ht="122.1" customHeight="1">
+      <c r="A14" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:250" ht="135.94999999999999" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:250" ht="144.94999999999999" customHeight="1">
+      <c r="A16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="1:250" ht="138.94999999999999" customHeight="1">
+      <c r="A17" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="1:250" ht="143.1" customHeight="1">
+      <c r="A18" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="1:250" ht="180">
+      <c r="A19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
+      <c r="BN20"/>
+      <c r="BO20"/>
+      <c r="BP20"/>
+      <c r="BQ20"/>
+      <c r="BR20"/>
+      <c r="BS20"/>
+      <c r="BT20"/>
+      <c r="BU20"/>
+      <c r="BV20"/>
+      <c r="BW20"/>
+      <c r="BX20"/>
+      <c r="BY20"/>
+      <c r="BZ20"/>
+      <c r="CA20"/>
+      <c r="CB20"/>
+      <c r="CC20"/>
+      <c r="CD20"/>
+      <c r="CE20"/>
+      <c r="CF20"/>
+      <c r="CG20"/>
+      <c r="CH20"/>
+      <c r="CI20"/>
+      <c r="CJ20"/>
+      <c r="CK20"/>
+      <c r="CL20"/>
+      <c r="CM20"/>
+      <c r="CN20"/>
+      <c r="CO20"/>
+      <c r="CP20"/>
+      <c r="CQ20"/>
+      <c r="CR20"/>
+      <c r="CS20"/>
+      <c r="CT20"/>
+      <c r="CU20"/>
+      <c r="CV20"/>
+      <c r="CW20"/>
+      <c r="CX20"/>
+      <c r="CY20"/>
+      <c r="CZ20"/>
+      <c r="DA20"/>
+      <c r="DB20"/>
+      <c r="DC20"/>
+      <c r="DD20"/>
+      <c r="DE20"/>
+      <c r="DF20"/>
+      <c r="DG20"/>
+      <c r="DH20"/>
+      <c r="DI20"/>
+      <c r="DJ20"/>
+      <c r="DK20"/>
+      <c r="DL20"/>
+      <c r="DM20"/>
+      <c r="DN20"/>
+      <c r="DO20"/>
+      <c r="DP20"/>
+      <c r="DQ20"/>
+      <c r="DR20"/>
+      <c r="DS20"/>
+      <c r="DT20"/>
+      <c r="DU20"/>
+      <c r="DV20"/>
+      <c r="DW20"/>
+      <c r="DX20"/>
+      <c r="DY20"/>
+      <c r="DZ20"/>
+      <c r="EA20"/>
+      <c r="EB20"/>
+      <c r="EC20"/>
+      <c r="ED20"/>
+      <c r="EE20"/>
+      <c r="EF20"/>
+      <c r="EG20"/>
+      <c r="EH20"/>
+      <c r="EI20"/>
+      <c r="EJ20"/>
+      <c r="EK20"/>
+      <c r="EL20"/>
+      <c r="EM20"/>
+      <c r="EN20"/>
+      <c r="EO20"/>
+      <c r="EP20"/>
+      <c r="EQ20"/>
+      <c r="ER20"/>
+      <c r="ES20"/>
+      <c r="ET20"/>
+      <c r="EU20"/>
+      <c r="EV20"/>
+      <c r="EW20"/>
+      <c r="EX20"/>
+      <c r="EY20"/>
+      <c r="EZ20"/>
+      <c r="FA20"/>
+      <c r="FB20"/>
+      <c r="FC20"/>
+      <c r="FD20"/>
+      <c r="FE20"/>
+      <c r="FF20"/>
+      <c r="FG20"/>
+      <c r="FH20"/>
+      <c r="FI20"/>
+      <c r="FJ20"/>
+      <c r="FK20"/>
+      <c r="FL20"/>
+      <c r="FM20"/>
+      <c r="FN20"/>
+      <c r="FO20"/>
+      <c r="FP20"/>
+      <c r="FQ20"/>
+      <c r="FR20"/>
+      <c r="FS20"/>
+      <c r="FT20"/>
+      <c r="FU20"/>
+      <c r="FV20"/>
+      <c r="FW20"/>
+      <c r="FX20"/>
+      <c r="FY20"/>
+      <c r="FZ20"/>
+      <c r="GA20"/>
+      <c r="GB20"/>
+      <c r="GC20"/>
+      <c r="GD20"/>
+      <c r="GE20"/>
+      <c r="GF20"/>
+      <c r="GG20"/>
+      <c r="GH20"/>
+      <c r="GI20"/>
+      <c r="GJ20"/>
+      <c r="GK20"/>
+      <c r="GL20"/>
+      <c r="GM20"/>
+      <c r="GN20"/>
+      <c r="GO20"/>
+      <c r="GP20"/>
+      <c r="GQ20"/>
+      <c r="GR20"/>
+      <c r="GS20"/>
+      <c r="GT20"/>
+      <c r="GU20"/>
+      <c r="GV20"/>
+      <c r="GW20"/>
+      <c r="GX20"/>
+      <c r="GY20"/>
+      <c r="GZ20"/>
+      <c r="HA20"/>
+      <c r="HB20"/>
+      <c r="HC20"/>
+      <c r="HD20"/>
+      <c r="HE20"/>
+      <c r="HF20"/>
+      <c r="HG20"/>
+      <c r="HH20"/>
+      <c r="HI20"/>
+      <c r="HJ20"/>
+      <c r="HK20"/>
+      <c r="HL20"/>
+      <c r="HM20"/>
+      <c r="HN20"/>
+      <c r="HO20"/>
+      <c r="HP20"/>
+      <c r="HQ20"/>
+      <c r="HR20"/>
+      <c r="HS20"/>
+      <c r="HT20"/>
+      <c r="HU20"/>
+      <c r="HV20"/>
+      <c r="HW20"/>
+      <c r="HX20"/>
+      <c r="HY20"/>
+      <c r="HZ20"/>
+      <c r="IA20"/>
+      <c r="IB20"/>
+      <c r="IC20"/>
+      <c r="ID20"/>
+      <c r="IE20"/>
+      <c r="IF20"/>
+      <c r="IG20"/>
+      <c r="IH20"/>
+      <c r="II20"/>
+      <c r="IJ20"/>
+      <c r="IK20"/>
+      <c r="IL20"/>
+      <c r="IM20"/>
+      <c r="IN20"/>
+      <c r="IO20"/>
+      <c r="IP20"/>
+    </row>
+    <row r="21" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
     </row>
-    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
     </row>
-    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2985,12 +3512,22 @@
       <c r="E52" s="22"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E52"/>
   <phoneticPr fontId="11"/>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1"/>
     <hyperlink ref="D8" r:id="rId2"/>
     <hyperlink ref="D9" r:id="rId3"/>
     <hyperlink ref="D10" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
+    <hyperlink ref="D18" r:id="rId12"/>
+    <hyperlink ref="D19" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Upload Atmos (Key Properties only) for MIROC-ES2L and MIROC-ES2H, turn "on" to publish. And also citations and responsible_parites spreadsheets are updated.
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_miroc_citations.xlsx
+++ b/cmip6/citations/cmip6_miroc_citations.xlsx
@@ -19,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Citations!$A$1:$E$52</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -446,12 +446,36 @@
 DOI = {10.5194/gmd-4-845-2011}
 }</t>
   </si>
+  <si>
+    <t>Hajima_in.prep</t>
+  </si>
+  <si>
+    <t>Not yet available</t>
+  </si>
+  <si>
+    <t>Ito_2016</t>
+  </si>
+  <si>
+    <t>10.1016/j.polar.2015.11.002</t>
+  </si>
+  <si>
+    <t>Iti_Oikawa_2002</t>
+  </si>
+  <si>
+    <t>10.1016/S0304-3800(01)00473-2</t>
+  </si>
+  <si>
+    <t>Ito_Inatomi_2012, Ito_2016, Ito_Oikawa_2002</t>
+  </si>
+  <si>
+    <t>10.5194/bg-9-759-2012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -551,8 +575,34 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,6 +619,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -685,15 +741,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -797,10 +859,27 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
+    <cellStyle name="ハイパーリンク 2" xfId="3"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -2734,8 +2813,8 @@
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -3036,9 +3115,15 @@
       <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
+      <c r="A20" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
@@ -3288,23 +3373,35 @@
       <c r="IP20"/>
     </row>
     <row r="21" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="A21" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="39"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="A22" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="39"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:250" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="39"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>

</xml_diff>